<commit_message>
saving from hosting folder
</commit_message>
<xml_diff>
--- a/Образец модифицированного бланка.xlsx
+++ b/Образец модифицированного бланка.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="43">
   <si>
     <t>40</t>
   </si>
@@ -103,6 +103,51 @@
   </si>
   <si>
     <t>SUBART</t>
+  </si>
+  <si>
+    <t>TIAT164 - красный</t>
+  </si>
+  <si>
+    <t>Палантин женский</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>100% акрил</t>
+  </si>
+  <si>
+    <t>красный</t>
+  </si>
+  <si>
+    <t>Классический палантин благородного цвета. Отличный выбор для тех, кто хочет  разнообразить свой повседневный образ. Благодаря широкому крою, палантин прекрасно драпируется в разных вариантах, и… «вуаля!» – Вы смело можете использовать его в качестве накидки, гуляя по городу ранней осенью. По нижнему краю палантин украшен бахромой. Приятная на ощупь ткань не мнется. Изделие представлено в белом, черном, ярко–синем, лиловом, красном, бордовом, сером, горчичном цветах, а также актуальном в этом сезоне цвете под джинсу.Размеры: 57*180 см.</t>
+  </si>
+  <si>
+    <t>TIAT164 - бордовый</t>
+  </si>
+  <si>
+    <t>бордовый</t>
+  </si>
+  <si>
+    <t>TIAT164 - коричневый</t>
+  </si>
+  <si>
+    <t>коричневый</t>
+  </si>
+  <si>
+    <t>ZZ034 - белый</t>
+  </si>
+  <si>
+    <t>Зажим на женский платок</t>
+  </si>
+  <si>
+    <t>см, на упаковке</t>
+  </si>
+  <si>
+    <t>белый</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -180,9 +225,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -193,9 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -499,370 +552,463 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="14" width="7" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="32" width="14" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="25" style="4" customWidth="1"/>
+    <col min="8" max="14" width="7" style="4" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="10" style="4" customWidth="1"/>
+    <col min="17" max="32" width="14" style="4" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.9" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>5815</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>5815</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>5815</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>5815</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>5815</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>8500</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>8500</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>8500</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <v>8500</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <v>4220</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>4220</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <v>4220</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="2">
         <v>4220</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="2">
         <v>4220</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2">
+        <v>467</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="2">
+        <v>467</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2">
+        <v>467</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="8">
+        <v>200</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>